<commit_message>
Add support for shared strings
</commit_message>
<xml_diff>
--- a/spec/file/test.xlsx
+++ b/spec/file/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,6 +19,17 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Foo bar</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
@@ -29,6 +40,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -110,16 +122,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -127,13 +136,24 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" s="0" t="n">
         <v>1.1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="D3" s="0" t="n">
         <v>-56</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="0" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>